<commit_message>
Updated ppt; Updated Readme file (citations, methods, results, data, issues)
</commit_message>
<xml_diff>
--- a/Data/list_of_hosts.xlsx
+++ b/Data/list_of_hosts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaver\Documents\_Yale\Spring_2019\Comparative_Genomics\Final_project\finalproject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A499EB31-CA1A-4C75-A7A9-0B02D24CA2F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD8ACD2-7765-4FEC-AF72-DDFE2C04B117}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="6120" windowWidth="15375" windowHeight="7875" xr2:uid="{F220A59E-9B37-4CDC-938D-EF244F5C1D54}"/>
+    <workbookView xWindow="11610" yWindow="2445" windowWidth="15375" windowHeight="7875" xr2:uid="{F220A59E-9B37-4CDC-938D-EF244F5C1D54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>S Bongori NCTC12419</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>Chicken/Fowl</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -170,6 +179,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CCAA19E6-8519-469C-9E18-E55ADC77EFE2}" name="Table4" displayName="Table4" ref="C1:D22" totalsRowShown="0">
+  <autoFilter ref="C1:D22" xr:uid="{AEA3462D-E76B-428F-8C5B-AEECECD0B35D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{2D6E0E44-1546-43EC-BB77-43864E9EF371}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{E6D96156-D3BD-45F5-9582-8956F95996C6}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -469,180 +489,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C2B6C2-61E4-4424-80D7-F26B1A574170}">
-  <dimension ref="C1:F21"/>
+  <dimension ref="C1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C1" sqref="C1:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="F1" t="s">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
+      <c r="D9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="F12" t="s">
+      <c r="D13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="F13" t="s">
+      <c r="D14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="F14" t="s">
+      <c r="D15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="F16" t="s">
+      <c r="D17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>15</v>
       </c>
-      <c r="F17" t="s">
+      <c r="D18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>16</v>
       </c>
-      <c r="F18" t="s">
+      <c r="D19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>17</v>
       </c>
-      <c r="F19" t="s">
+      <c r="D20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="F20" t="s">
+      <c r="D21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>19</v>
       </c>
-      <c r="F21" t="s">
+      <c r="D22" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>